<commit_message>
Separated Optimizer class in two
OptSearcher only has static methods, Optimizer has to be instantiated
</commit_message>
<xml_diff>
--- a/Konzept.xlsx
+++ b/Konzept.xlsx
@@ -262,7 +262,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -275,9 +275,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -315,7 +315,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -387,7 +387,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -567,7 +567,7 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="18.5703125" customWidth="1"/>
   </cols>
@@ -799,7 +799,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -811,7 +811,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>